<commit_message>
logger added, SKU changed, cookies removed
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I5310\eclipse-workspace\Cucumber_Oct_23\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I5310\eclipse-workspace\SDET_Sameer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0E115B-50B4-4FF8-B6F4-81B81F1E0349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F73A5F5-8D89-48FB-8877-4F59988A3B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{03D5A7F2-CF5D-45C8-983B-7E9C5DD17D1A}"/>
   </bookViews>
@@ -36,12 +36,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Searchtext</t>
   </si>
   <si>
-    <t>Shiirtss</t>
+    <t>Shirts</t>
+  </si>
+  <si>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>MSP84FX14025</t>
+  </si>
+  <si>
+    <t>XL</t>
   </si>
 </sst>
 </file>
@@ -393,22 +411,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1B14B8-9BCD-46D3-AF74-C1B714A86204}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.36328125" customWidth="1"/>
+    <col min="2" max="2" width="16.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel file input added
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I5310\eclipse-workspace\SDET_Sameer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F73A5F5-8D89-48FB-8877-4F59988A3B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD191C5-A917-4DC5-96A0-9F94A9A2A031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{03D5A7F2-CF5D-45C8-983B-7E9C5DD17D1A}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Searchtext</t>
   </si>
   <si>
-    <t>Shirts</t>
-  </si>
-  <si>
     <t>SKU</t>
   </si>
   <si>
@@ -53,13 +50,22 @@
     <t>Size</t>
   </si>
   <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>MSP84FX14025</t>
-  </si>
-  <si>
-    <t>XL</t>
+    <t>red shirts</t>
+  </si>
+  <si>
+    <t>MSP64LT20025</t>
+  </si>
+  <si>
+    <t>Navy</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Product name</t>
+  </si>
+  <si>
+    <t>AWEARNESS Kenneth Cole</t>
   </si>
 </sst>
 </file>
@@ -411,44 +417,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1B14B8-9BCD-46D3-AF74-C1B714A86204}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.36328125" customWidth="1"/>
     <col min="2" max="2" width="16.08984375" customWidth="1"/>
+    <col min="5" max="5" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>